<commit_message>
Add learning part Visualization
</commit_message>
<xml_diff>
--- a/Learning/Exam_PL_300.xlsx
+++ b/Learning/Exam_PL_300.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Powerbi\Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54179535-41A2-4D5A-B1ED-071B4A467C53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4BD0F85-5127-4FC2-9119-7A92A852C5F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="6" activeTab="9" xr2:uid="{FDBA2C08-A540-44DB-960E-EBA441ABF6B7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="6" activeTab="6" xr2:uid="{FDBA2C08-A540-44DB-960E-EBA441ABF6B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Exam" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="6x.Revision Prepare data" sheetId="7" r:id="rId8"/>
     <sheet name="7.Visualization" sheetId="8" r:id="rId9"/>
     <sheet name="8.format table and matrix" sheetId="9" r:id="rId10"/>
+    <sheet name="1.Group " sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="114">
   <si>
     <t xml:space="preserve">Topic </t>
   </si>
@@ -369,6 +370,27 @@
   </si>
   <si>
     <t>https://learn.microsoft.com/fr-fr/power-bi/natural-language/q-and-a-best-practices</t>
+  </si>
+  <si>
+    <t>Udemy</t>
+  </si>
+  <si>
+    <t>Use group (Bin and List)</t>
+  </si>
+  <si>
+    <t>List or Bin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bin size or bin count </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Count give you the number or round </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bin size is the numerical value of the size </t>
+  </si>
+  <si>
+    <t>List will aggregate in groups</t>
   </si>
 </sst>
 </file>
@@ -443,11 +465,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -922,6 +943,50 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>114</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>151281</xdr:colOff>
+      <xdr:row>132</xdr:row>
+      <xdr:rowOff>20561</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{234B8D42-B0E8-FFC8-051B-DC7625E883CB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="342900" y="21008340"/>
+          <a:ext cx="8952381" cy="3152381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2440,6 +2505,99 @@
         <a:xfrm>
           <a:off x="1" y="2659380"/>
           <a:ext cx="7139940" cy="3048589"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>601981</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>152401</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>502921</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>26385</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2FE41D10-4251-EC93-89C3-F8FDA91AB0DE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="601981" y="518161"/>
+          <a:ext cx="2948940" cy="2617184"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>37</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>501915</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>109997</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA352A4A-EE93-FB0A-A152-45AFA6BD27CC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7018057" y="3429000"/>
+          <a:ext cx="4418558" cy="2167397"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2768,10 +2926,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C494E46-834D-4E41-B7EB-D66A95B60955}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2813,7 +2971,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
+      <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="2">
@@ -2839,7 +2997,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
+      <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" s="2">
@@ -3009,7 +3167,7 @@
       <c r="A10">
         <v>1</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="4">
         <v>45</v>
       </c>
       <c r="C10" t="s">
@@ -3072,7 +3230,7 @@
       <c r="A13">
         <v>1</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="4">
         <v>55</v>
       </c>
       <c r="C13" t="s">
@@ -3155,7 +3313,7 @@
       <c r="A17">
         <v>1</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="5" t="s">
         <v>69</v>
       </c>
       <c r="C17" t="s">
@@ -3175,7 +3333,7 @@
       <c r="A18">
         <v>1</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18" s="7">
         <v>53</v>
       </c>
       <c r="C18" t="s">
@@ -3195,7 +3353,7 @@
       <c r="A19">
         <v>1</v>
       </c>
-      <c r="B19" s="7">
+      <c r="B19" s="6">
         <v>13</v>
       </c>
       <c r="C19" t="s">
@@ -3209,7 +3367,7 @@
       <c r="A20">
         <v>1</v>
       </c>
-      <c r="B20" s="7">
+      <c r="B20" s="6">
         <v>14</v>
       </c>
       <c r="C20" t="s">
@@ -3217,6 +3375,23 @@
       </c>
       <c r="E20" t="s">
         <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21">
+        <v>15</v>
+      </c>
+      <c r="C21" t="s">
+        <v>107</v>
+      </c>
+      <c r="D21" t="s">
+        <v>108</v>
+      </c>
+      <c r="E21" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -3251,12 +3426,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCC672AC-D1B6-47E6-892E-3F15F7876283}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="P27" sqref="P27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9C50580-9199-474A-A14F-BCBD7014DAFB}">
+  <dimension ref="H4:K7"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="8" max="8" width="22.33203125" customWidth="1"/>
+    <col min="11" max="11" width="39.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="8:11" x14ac:dyDescent="0.3">
+      <c r="H4" t="s">
+        <v>109</v>
+      </c>
+      <c r="K4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="8:11" x14ac:dyDescent="0.3">
+      <c r="H6" t="s">
+        <v>113</v>
+      </c>
+      <c r="K6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="8:11" x14ac:dyDescent="0.3">
+      <c r="K7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -3297,8 +3513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FC9650C-4DB4-4607-9B9E-5E596308CD52}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="F92" sqref="F92"/>
+    <sheetView topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="G123" sqref="G123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3409,20 +3625,20 @@
       </c>
     </row>
     <row r="3" spans="2:3" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="23" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="34" spans="2:3" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="3" t="s">
         <v>31</v>
       </c>
     </row>
@@ -3450,7 +3666,7 @@
       <c r="A1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>40</v>
       </c>
     </row>
@@ -3458,7 +3674,7 @@
       <c r="A3" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>41</v>
       </c>
     </row>
@@ -3466,7 +3682,7 @@
       <c r="A6" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>43</v>
       </c>
     </row>
@@ -3500,7 +3716,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F16E173E-E4B9-4926-AA22-6BEA3E5D072A}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -3569,15 +3785,15 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="3" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="3" t="s">
         <v>61</v>
       </c>
     </row>
@@ -3601,7 +3817,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2582188-C7C0-47B3-9136-8DEAE583249A}">
   <dimension ref="A1:M85"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N93" sqref="N93"/>
     </sheetView>
   </sheetViews>
@@ -3651,6 +3867,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BF0C278202264D448BAD329AD0320563" ma:contentTypeVersion="8" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="42e1ada70272376831707128d7b50210">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="177883a4-d7d8-459f-8663-1478538f782e" xmlns:ns4="c7ca6911-0430-472b-8881-b1995898bd6d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c17d8125c14eff56a8d9e5ca22ee7c34" ns3:_="" ns4:_="">
     <xsd:import namespace="177883a4-d7d8-459f-8663-1478538f782e"/>
@@ -3839,15 +4064,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -3857,6 +4073,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF401ABE-1263-486E-A9ED-21D88EB75D80}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5DEAFC1-8861-4F66-BE16-5B80E1B802AF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3871,14 +4095,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF401ABE-1263-486E-A9ED-21D88EB75D80}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>